<commit_message>
Fixed encoding and added status
</commit_message>
<xml_diff>
--- a/resources/whist_20170926.xlsx
+++ b/resources/whist_20170926.xlsx
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="77" uniqueCount="29">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="78" uniqueCount="30">
   <si>
     <t>Games</t>
   </si>
@@ -108,6 +108,9 @@
   </si>
   <si>
     <t>SELVMAKKER</t>
+  </si>
+  <si>
+    <t>STOP</t>
   </si>
 </sst>
 </file>
@@ -477,8 +480,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:Q71"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" zoomScale="140" zoomScaleNormal="140" workbookViewId="0">
-      <selection activeCell="C3" sqref="C3"/>
+    <sheetView tabSelected="1" topLeftCell="A19" zoomScale="140" zoomScaleNormal="140" workbookViewId="0">
+      <selection activeCell="A31" sqref="A31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -980,7 +983,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="17" spans="3:17" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:17" x14ac:dyDescent="0.25">
       <c r="C17">
         <v>6</v>
       </c>
@@ -1013,7 +1016,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="18" spans="3:17" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:17" x14ac:dyDescent="0.25">
       <c r="C18">
         <v>-32</v>
       </c>
@@ -1046,7 +1049,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="19" spans="3:17" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:17" x14ac:dyDescent="0.25">
       <c r="C19">
         <v>8</v>
       </c>
@@ -1076,7 +1079,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="20" spans="3:17" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:17" x14ac:dyDescent="0.25">
       <c r="C20">
         <v>2</v>
       </c>
@@ -1112,7 +1115,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="21" spans="3:17" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:17" x14ac:dyDescent="0.25">
       <c r="C21">
         <v>-16</v>
       </c>
@@ -1152,7 +1155,7 @@
         <v>2.2400000000000002</v>
       </c>
     </row>
-    <row r="22" spans="3:17" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:17" x14ac:dyDescent="0.25">
       <c r="C22">
         <v>-16</v>
       </c>
@@ -1188,7 +1191,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="23" spans="3:17" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:17" x14ac:dyDescent="0.25">
       <c r="C23">
         <v>4</v>
       </c>
@@ -1218,7 +1221,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="24" spans="3:17" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:17" x14ac:dyDescent="0.25">
       <c r="C24">
         <v>6</v>
       </c>
@@ -1245,7 +1248,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="25" spans="3:17" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:17" x14ac:dyDescent="0.25">
       <c r="C25">
         <v>-2</v>
       </c>
@@ -1278,7 +1281,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="26" spans="3:17" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:17" x14ac:dyDescent="0.25">
       <c r="C26">
         <v>-12</v>
       </c>
@@ -1311,7 +1314,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="27" spans="3:17" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:17" x14ac:dyDescent="0.25">
       <c r="C27">
         <v>6</v>
       </c>
@@ -1335,7 +1338,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="28" spans="3:17" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:17" x14ac:dyDescent="0.25">
       <c r="C28">
         <v>-8</v>
       </c>
@@ -1368,7 +1371,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="29" spans="3:17" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:17" x14ac:dyDescent="0.25">
       <c r="C29">
         <v>4</v>
       </c>
@@ -1401,7 +1404,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="30" spans="3:17" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:17" x14ac:dyDescent="0.25">
       <c r="C30">
         <v>4</v>
       </c>
@@ -1425,14 +1428,17 @@
         <v>4</v>
       </c>
     </row>
-    <row r="31" spans="3:17" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A31" t="s">
+        <v>29</v>
+      </c>
       <c r="G31">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="I31" s="5"/>
     </row>
-    <row r="32" spans="3:17" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:17" x14ac:dyDescent="0.25">
       <c r="G32">
         <f t="shared" si="0"/>
         <v>0</v>
@@ -1694,8 +1700,8 @@
           <x14:colorLow rgb="FFD00000"/>
           <x14:sparklines>
             <x14:sparkline>
-              <xm:f>Sheet1!K6:K52</xm:f>
-              <xm:sqref>I24</xm:sqref>
+              <xm:f>Sheet1!K6:K23</xm:f>
+              <xm:sqref>I26</xm:sqref>
             </x14:sparkline>
           </x14:sparklines>
         </x14:sparklineGroup>
@@ -1710,8 +1716,8 @@
           <x14:colorLow rgb="FFD00000"/>
           <x14:sparklines>
             <x14:sparkline>
-              <xm:f>Sheet1!K6:K23</xm:f>
-              <xm:sqref>I26</xm:sqref>
+              <xm:f>Sheet1!K6:K52</xm:f>
+              <xm:sqref>I24</xm:sqref>
             </x14:sparkline>
           </x14:sparklines>
         </x14:sparklineGroup>

</xml_diff>